<commit_message>
Update vertalingen (deel 2)
#30
</commit_message>
<xml_diff>
--- a/alienSpecies/inst/extdata/translations_v23-05-24.xlsx
+++ b/alienSpecies/inst/extdata/translations_v23-05-24.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bram_dhondt\Documents\GitHub\alien-species-portal\alienSpecies\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A24B49F7-0852-4995-B002-9600BC936F1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9253A1DA-410E-4C3C-BC7A-5054D597DE1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="987" uniqueCount="858">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="998" uniqueCount="866">
   <si>
     <t>title_id</t>
   </si>
@@ -1386,9 +1386,6 @@
     <t>combineRegions</t>
   </si>
   <si>
-    <t>Combineer alle geselecteerde regio’s in de trend grafiek</t>
-  </si>
-  <si>
     <t>Combine all selected regions in the trend graph</t>
   </si>
   <si>
@@ -2448,30 +2445,18 @@
     <t>multipleRegions</t>
   </si>
   <si>
-    <t>Meer dan 1 regio</t>
-  </si>
-  <si>
-    <t>Multiple regions</t>
-  </si>
-  <si>
     <t>not selected</t>
   </si>
   <si>
     <t>niet geselecteerd</t>
   </si>
   <si>
-    <t>Not selected</t>
-  </si>
-  <si>
     <t>selected</t>
   </si>
   <si>
     <t>geselecteerd</t>
   </si>
   <si>
-    <t>Selected</t>
-  </si>
-  <si>
     <t>Ad hoc alien species checklist</t>
   </si>
   <si>
@@ -2598,7 +2583,46 @@
     <t>Unknown (not specified)</t>
   </si>
   <si>
-    <t>Plusieurs Régions</t>
+    <t>Combinez toutes les régions sélectionnées dans le graphique de tendance</t>
+  </si>
+  <si>
+    <t>Combineer alle geselecteerde regio’s in de trendgrafiek</t>
+  </si>
+  <si>
+    <t>non séléctionné</t>
+  </si>
+  <si>
+    <t>séléctionné</t>
+  </si>
+  <si>
+    <t>meer dan 1 gewest</t>
+  </si>
+  <si>
+    <t>région</t>
+  </si>
+  <si>
+    <t>plusieurs régions</t>
+  </si>
+  <si>
+    <t>multiple regions</t>
+  </si>
+  <si>
+    <t>Union couleur</t>
+  </si>
+  <si>
+    <t>Observation couleur</t>
+  </si>
+  <si>
+    <t>Observation</t>
+  </si>
+  <si>
+    <t>Figure</t>
+  </si>
+  <si>
+    <t>Union colour</t>
+  </si>
+  <si>
+    <t>Observation colour</t>
   </si>
 </sst>
 </file>
@@ -2919,16 +2943,16 @@
   <dimension ref="A1:G266"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D249" sqref="D249"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.44140625" customWidth="1"/>
-    <col min="3" max="3" width="3.5546875" customWidth="1"/>
-    <col min="4" max="4" width="40.5546875" customWidth="1"/>
-    <col min="5" max="5" width="1.33203125" customWidth="1"/>
+    <col min="2" max="2" width="93.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="64.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="122.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="89.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="90.77734375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="65.109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -4706,1688 +4730,1721 @@
         <v>452</v>
       </c>
       <c r="B133" t="s">
+        <v>853</v>
+      </c>
+      <c r="D133" t="s">
+        <v>852</v>
+      </c>
+      <c r="F133" t="s">
         <v>453</v>
-      </c>
-      <c r="F133" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
+        <v>454</v>
+      </c>
+      <c r="B138" t="s">
         <v>455</v>
       </c>
-      <c r="B138" t="s">
+      <c r="D138" t="s">
         <v>456</v>
       </c>
-      <c r="D138" t="s">
+      <c r="F138" t="s">
         <v>457</v>
-      </c>
-      <c r="F138" t="s">
-        <v>458</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
+        <v>458</v>
+      </c>
+      <c r="B139" t="s">
         <v>459</v>
       </c>
-      <c r="B139" t="s">
+      <c r="D139" t="s">
         <v>460</v>
       </c>
-      <c r="D139" t="s">
+      <c r="F139" t="s">
         <v>461</v>
-      </c>
-      <c r="F139" t="s">
-        <v>462</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
+        <v>462</v>
+      </c>
+      <c r="B140" t="s">
         <v>463</v>
       </c>
-      <c r="B140" t="s">
+      <c r="D140" t="s">
         <v>464</v>
       </c>
-      <c r="D140" t="s">
-        <v>465</v>
-      </c>
       <c r="F140" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
+        <v>465</v>
+      </c>
+      <c r="B141" t="s">
         <v>466</v>
       </c>
-      <c r="B141" t="s">
+      <c r="D141" t="s">
         <v>467</v>
       </c>
-      <c r="D141" t="s">
+      <c r="F141" t="s">
         <v>468</v>
-      </c>
-      <c r="F141" t="s">
-        <v>469</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
+        <v>469</v>
+      </c>
+      <c r="B142" t="s">
         <v>470</v>
       </c>
-      <c r="B142" t="s">
+      <c r="D142" t="s">
         <v>471</v>
       </c>
-      <c r="D142" t="s">
-        <v>472</v>
-      </c>
       <c r="F142" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
+        <v>472</v>
+      </c>
+      <c r="B143" t="s">
         <v>473</v>
       </c>
-      <c r="B143" t="s">
+      <c r="D143" t="s">
         <v>474</v>
       </c>
-      <c r="D143" t="s">
+      <c r="F143" t="s">
         <v>475</v>
-      </c>
-      <c r="F143" t="s">
-        <v>476</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
+        <v>476</v>
+      </c>
+      <c r="B144" t="s">
         <v>477</v>
       </c>
-      <c r="B144" t="s">
+      <c r="D144" t="s">
         <v>478</v>
       </c>
-      <c r="D144" t="s">
+      <c r="F144" t="s">
         <v>479</v>
-      </c>
-      <c r="F144" t="s">
-        <v>480</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
+        <v>480</v>
+      </c>
+      <c r="B145" t="s">
         <v>481</v>
       </c>
-      <c r="B145" t="s">
+      <c r="D145" t="s">
         <v>482</v>
       </c>
-      <c r="D145" t="s">
+      <c r="F145" t="s">
         <v>483</v>
-      </c>
-      <c r="F145" t="s">
-        <v>484</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
+        <v>484</v>
+      </c>
+      <c r="B146" t="s">
         <v>485</v>
       </c>
-      <c r="B146" t="s">
+      <c r="D146" t="s">
         <v>486</v>
       </c>
-      <c r="D146" t="s">
+      <c r="F146" t="s">
         <v>487</v>
-      </c>
-      <c r="F146" t="s">
-        <v>488</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
+        <v>488</v>
+      </c>
+      <c r="B147" t="s">
         <v>489</v>
       </c>
-      <c r="B147" t="s">
+      <c r="D147" t="s">
         <v>490</v>
       </c>
-      <c r="D147" t="s">
+      <c r="F147" t="s">
         <v>491</v>
-      </c>
-      <c r="F147" t="s">
-        <v>492</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
+        <v>492</v>
+      </c>
+      <c r="B148" t="s">
         <v>493</v>
       </c>
-      <c r="B148" t="s">
+      <c r="D148" t="s">
         <v>494</v>
       </c>
-      <c r="D148" t="s">
+      <c r="F148" t="s">
         <v>495</v>
-      </c>
-      <c r="F148" t="s">
-        <v>496</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
+        <v>496</v>
+      </c>
+      <c r="B149" t="s">
         <v>497</v>
       </c>
-      <c r="B149" t="s">
+      <c r="D149" t="s">
         <v>498</v>
       </c>
-      <c r="D149" t="s">
+      <c r="F149" t="s">
         <v>499</v>
-      </c>
-      <c r="F149" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
+        <v>500</v>
+      </c>
+      <c r="B150" t="s">
         <v>501</v>
       </c>
-      <c r="B150" t="s">
+      <c r="D150" t="s">
         <v>502</v>
       </c>
-      <c r="D150" t="s">
+      <c r="F150" t="s">
         <v>503</v>
-      </c>
-      <c r="F150" t="s">
-        <v>504</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
+        <v>504</v>
+      </c>
+      <c r="B151" t="s">
         <v>505</v>
       </c>
-      <c r="B151" t="s">
+      <c r="D151" t="s">
         <v>506</v>
       </c>
-      <c r="D151" t="s">
+      <c r="F151" t="s">
         <v>507</v>
-      </c>
-      <c r="F151" t="s">
-        <v>508</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
+        <v>508</v>
+      </c>
+      <c r="B152" t="s">
         <v>509</v>
       </c>
-      <c r="B152" t="s">
+      <c r="D152" t="s">
         <v>510</v>
       </c>
-      <c r="D152" t="s">
+      <c r="F152" t="s">
         <v>511</v>
-      </c>
-      <c r="F152" t="s">
-        <v>512</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
+        <v>512</v>
+      </c>
+      <c r="B153" t="s">
         <v>513</v>
       </c>
-      <c r="B153" t="s">
+      <c r="D153" t="s">
         <v>514</v>
       </c>
-      <c r="D153" t="s">
+      <c r="F153" t="s">
         <v>515</v>
-      </c>
-      <c r="F153" t="s">
-        <v>516</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
+        <v>516</v>
+      </c>
+      <c r="B154" t="s">
         <v>517</v>
       </c>
-      <c r="B154" t="s">
+      <c r="D154" t="s">
         <v>518</v>
       </c>
-      <c r="D154" t="s">
+      <c r="F154" t="s">
         <v>519</v>
-      </c>
-      <c r="F154" t="s">
-        <v>520</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
+        <v>520</v>
+      </c>
+      <c r="B155" t="s">
         <v>521</v>
       </c>
-      <c r="B155" t="s">
+      <c r="D155" t="s">
         <v>522</v>
       </c>
-      <c r="D155" t="s">
+      <c r="F155" t="s">
         <v>523</v>
-      </c>
-      <c r="F155" t="s">
-        <v>524</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
+        <v>524</v>
+      </c>
+      <c r="B156" t="s">
         <v>525</v>
       </c>
-      <c r="B156" t="s">
+      <c r="D156" t="s">
         <v>526</v>
       </c>
-      <c r="D156" t="s">
+      <c r="F156" t="s">
         <v>527</v>
-      </c>
-      <c r="F156" t="s">
-        <v>528</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
+        <v>528</v>
+      </c>
+      <c r="B157" t="s">
         <v>529</v>
       </c>
-      <c r="B157" t="s">
+      <c r="D157" t="s">
         <v>530</v>
       </c>
-      <c r="D157" t="s">
+      <c r="F157" t="s">
         <v>531</v>
-      </c>
-      <c r="F157" t="s">
-        <v>532</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
+        <v>532</v>
+      </c>
+      <c r="B158" t="s">
         <v>533</v>
       </c>
-      <c r="B158" t="s">
+      <c r="D158" t="s">
         <v>534</v>
       </c>
-      <c r="D158" t="s">
+      <c r="F158" t="s">
         <v>535</v>
-      </c>
-      <c r="F158" t="s">
-        <v>536</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
+        <v>536</v>
+      </c>
+      <c r="B159" t="s">
         <v>537</v>
       </c>
-      <c r="B159" t="s">
+      <c r="D159" t="s">
         <v>538</v>
       </c>
-      <c r="D159" t="s">
-        <v>539</v>
-      </c>
       <c r="F159" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
+        <v>539</v>
+      </c>
+      <c r="B160" t="s">
         <v>540</v>
       </c>
-      <c r="B160" t="s">
+      <c r="D160" t="s">
         <v>541</v>
       </c>
-      <c r="D160" t="s">
+      <c r="F160" t="s">
         <v>542</v>
-      </c>
-      <c r="F160" t="s">
-        <v>543</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
+        <v>543</v>
+      </c>
+      <c r="B161" t="s">
         <v>544</v>
       </c>
-      <c r="B161" t="s">
+      <c r="D161" t="s">
         <v>545</v>
       </c>
-      <c r="D161" t="s">
+      <c r="F161" t="s">
         <v>546</v>
-      </c>
-      <c r="F161" t="s">
-        <v>547</v>
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
+        <v>547</v>
+      </c>
+      <c r="B162" t="s">
         <v>548</v>
       </c>
-      <c r="B162" t="s">
+      <c r="D162" t="s">
         <v>549</v>
       </c>
-      <c r="D162" t="s">
+      <c r="F162" t="s">
         <v>550</v>
-      </c>
-      <c r="F162" t="s">
-        <v>551</v>
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
+        <v>551</v>
+      </c>
+      <c r="B163" t="s">
         <v>552</v>
       </c>
-      <c r="B163" t="s">
+      <c r="D163" t="s">
         <v>553</v>
       </c>
-      <c r="D163" t="s">
+      <c r="F163" t="s">
         <v>554</v>
-      </c>
-      <c r="F163" t="s">
-        <v>555</v>
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
+        <v>555</v>
+      </c>
+      <c r="B164" t="s">
         <v>556</v>
       </c>
-      <c r="B164" t="s">
+      <c r="D164" t="s">
         <v>557</v>
       </c>
-      <c r="D164" t="s">
+      <c r="F164" t="s">
         <v>558</v>
-      </c>
-      <c r="F164" t="s">
-        <v>559</v>
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
+        <v>559</v>
+      </c>
+      <c r="B165" t="s">
         <v>560</v>
       </c>
-      <c r="B165" t="s">
+      <c r="D165" t="s">
         <v>561</v>
       </c>
-      <c r="D165" t="s">
+      <c r="F165" t="s">
         <v>562</v>
-      </c>
-      <c r="F165" t="s">
-        <v>563</v>
       </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
+        <v>563</v>
+      </c>
+      <c r="B166" t="s">
         <v>564</v>
       </c>
-      <c r="B166" t="s">
+      <c r="D166" t="s">
         <v>565</v>
       </c>
-      <c r="D166" t="s">
+      <c r="F166" t="s">
         <v>566</v>
-      </c>
-      <c r="F166" t="s">
-        <v>567</v>
       </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
+        <v>567</v>
+      </c>
+      <c r="B167" t="s">
         <v>568</v>
       </c>
-      <c r="B167" t="s">
+      <c r="D167" t="s">
         <v>569</v>
       </c>
-      <c r="D167" t="s">
+      <c r="F167" t="s">
         <v>570</v>
-      </c>
-      <c r="F167" t="s">
-        <v>571</v>
       </c>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
+        <v>571</v>
+      </c>
+      <c r="B168" t="s">
         <v>572</v>
       </c>
-      <c r="B168" t="s">
+      <c r="D168" t="s">
         <v>573</v>
       </c>
-      <c r="D168" t="s">
+      <c r="F168" t="s">
         <v>574</v>
-      </c>
-      <c r="F168" t="s">
-        <v>575</v>
       </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
+        <v>575</v>
+      </c>
+      <c r="B169" t="s">
         <v>576</v>
       </c>
-      <c r="B169" t="s">
+      <c r="D169" t="s">
         <v>577</v>
       </c>
-      <c r="D169" t="s">
+      <c r="F169" t="s">
         <v>578</v>
-      </c>
-      <c r="F169" t="s">
-        <v>579</v>
       </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
+        <v>579</v>
+      </c>
+      <c r="B170" t="s">
         <v>580</v>
       </c>
-      <c r="B170" t="s">
+      <c r="D170" t="s">
         <v>581</v>
       </c>
-      <c r="D170" t="s">
+      <c r="F170" t="s">
         <v>582</v>
-      </c>
-      <c r="F170" t="s">
-        <v>583</v>
       </c>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
+        <v>583</v>
+      </c>
+      <c r="B171" t="s">
         <v>584</v>
       </c>
-      <c r="B171" t="s">
+      <c r="D171" t="s">
         <v>585</v>
       </c>
-      <c r="D171" t="s">
+      <c r="F171" t="s">
         <v>586</v>
-      </c>
-      <c r="F171" t="s">
-        <v>587</v>
       </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
+        <v>587</v>
+      </c>
+      <c r="B172" t="s">
         <v>588</v>
       </c>
-      <c r="B172" t="s">
+      <c r="D172" t="s">
         <v>589</v>
       </c>
-      <c r="D172" t="s">
+      <c r="F172" t="s">
         <v>590</v>
-      </c>
-      <c r="F172" t="s">
-        <v>591</v>
       </c>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
+        <v>591</v>
+      </c>
+      <c r="B173" t="s">
         <v>592</v>
       </c>
-      <c r="B173" t="s">
+      <c r="D173" t="s">
         <v>593</v>
       </c>
-      <c r="D173" t="s">
+      <c r="F173" t="s">
         <v>594</v>
-      </c>
-      <c r="F173" t="s">
-        <v>595</v>
       </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
+        <v>595</v>
+      </c>
+      <c r="B174" t="s">
         <v>596</v>
       </c>
-      <c r="B174" t="s">
+      <c r="D174" t="s">
         <v>597</v>
       </c>
-      <c r="D174" t="s">
+      <c r="F174" t="s">
         <v>598</v>
-      </c>
-      <c r="F174" t="s">
-        <v>599</v>
       </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
+        <v>599</v>
+      </c>
+      <c r="B175" t="s">
         <v>600</v>
       </c>
-      <c r="B175" t="s">
+      <c r="D175" t="s">
         <v>601</v>
       </c>
-      <c r="D175" t="s">
+      <c r="F175" t="s">
         <v>602</v>
-      </c>
-      <c r="F175" t="s">
-        <v>603</v>
       </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
+        <v>603</v>
+      </c>
+      <c r="B176" t="s">
         <v>604</v>
       </c>
-      <c r="B176" t="s">
+      <c r="D176" t="s">
         <v>605</v>
       </c>
-      <c r="D176" t="s">
+      <c r="F176" t="s">
         <v>606</v>
-      </c>
-      <c r="F176" t="s">
-        <v>607</v>
       </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
+        <v>607</v>
+      </c>
+      <c r="B177" t="s">
         <v>608</v>
       </c>
-      <c r="B177" t="s">
+      <c r="D177" t="s">
         <v>609</v>
       </c>
-      <c r="D177" t="s">
+      <c r="F177" t="s">
         <v>610</v>
-      </c>
-      <c r="F177" t="s">
-        <v>611</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
+        <v>611</v>
+      </c>
+      <c r="B178" t="s">
         <v>612</v>
       </c>
-      <c r="B178" t="s">
+      <c r="D178" t="s">
         <v>613</v>
       </c>
-      <c r="D178" t="s">
+      <c r="F178" t="s">
         <v>614</v>
-      </c>
-      <c r="F178" t="s">
-        <v>615</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
+        <v>615</v>
+      </c>
+      <c r="B179" t="s">
         <v>616</v>
       </c>
-      <c r="B179" t="s">
+      <c r="D179" t="s">
         <v>617</v>
       </c>
-      <c r="D179" t="s">
+      <c r="F179" t="s">
         <v>618</v>
-      </c>
-      <c r="F179" t="s">
-        <v>619</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
+        <v>619</v>
+      </c>
+      <c r="B180" t="s">
         <v>620</v>
       </c>
-      <c r="B180" t="s">
+      <c r="D180" t="s">
         <v>621</v>
       </c>
-      <c r="D180" t="s">
+      <c r="F180" t="s">
         <v>622</v>
-      </c>
-      <c r="F180" t="s">
-        <v>623</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
+        <v>623</v>
+      </c>
+      <c r="B181" t="s">
         <v>624</v>
       </c>
-      <c r="B181" t="s">
+      <c r="D181" t="s">
         <v>625</v>
       </c>
-      <c r="D181" t="s">
+      <c r="F181" t="s">
         <v>626</v>
-      </c>
-      <c r="F181" t="s">
-        <v>627</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
+        <v>627</v>
+      </c>
+      <c r="B182" t="s">
         <v>628</v>
       </c>
-      <c r="B182" t="s">
+      <c r="D182" t="s">
         <v>629</v>
       </c>
-      <c r="D182" t="s">
+      <c r="F182" t="s">
         <v>630</v>
-      </c>
-      <c r="F182" t="s">
-        <v>631</v>
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
+        <v>631</v>
+      </c>
+      <c r="B183" t="s">
         <v>632</v>
       </c>
-      <c r="B183" t="s">
+      <c r="D183" t="s">
         <v>633</v>
       </c>
-      <c r="D183" t="s">
+      <c r="F183" t="s">
         <v>634</v>
-      </c>
-      <c r="F183" t="s">
-        <v>635</v>
       </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
+        <v>635</v>
+      </c>
+      <c r="B184" t="s">
         <v>636</v>
       </c>
-      <c r="B184" t="s">
+      <c r="D184" t="s">
         <v>637</v>
       </c>
-      <c r="D184" t="s">
+      <c r="F184" t="s">
         <v>638</v>
-      </c>
-      <c r="F184" t="s">
-        <v>639</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
+        <v>639</v>
+      </c>
+      <c r="B185" t="s">
         <v>640</v>
       </c>
-      <c r="B185" t="s">
+      <c r="D185" t="s">
         <v>641</v>
       </c>
-      <c r="D185" t="s">
+      <c r="F185" t="s">
         <v>642</v>
-      </c>
-      <c r="F185" t="s">
-        <v>643</v>
       </c>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
+        <v>643</v>
+      </c>
+      <c r="B186" t="s">
         <v>644</v>
       </c>
-      <c r="B186" t="s">
+      <c r="D186" t="s">
         <v>645</v>
       </c>
-      <c r="D186" t="s">
+      <c r="F186" t="s">
         <v>646</v>
-      </c>
-      <c r="F186" t="s">
-        <v>647</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
+        <v>647</v>
+      </c>
+      <c r="B187" t="s">
         <v>648</v>
       </c>
-      <c r="B187" t="s">
+      <c r="D187" t="s">
         <v>649</v>
       </c>
-      <c r="D187" t="s">
+      <c r="F187" t="s">
         <v>650</v>
-      </c>
-      <c r="F187" t="s">
-        <v>651</v>
       </c>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
+        <v>651</v>
+      </c>
+      <c r="B188" t="s">
         <v>652</v>
       </c>
-      <c r="B188" t="s">
+      <c r="D188" t="s">
         <v>653</v>
       </c>
-      <c r="D188" t="s">
+      <c r="F188" t="s">
         <v>654</v>
-      </c>
-      <c r="F188" t="s">
-        <v>655</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="B189" t="s">
-        <v>834</v>
+        <v>829</v>
       </c>
       <c r="D189" t="s">
-        <v>841</v>
+        <v>836</v>
       </c>
       <c r="F189" t="s">
-        <v>849</v>
+        <v>844</v>
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="B190" t="s">
-        <v>835</v>
+        <v>830</v>
       </c>
       <c r="D190" t="s">
-        <v>842</v>
+        <v>837</v>
       </c>
       <c r="F190" t="s">
-        <v>850</v>
+        <v>845</v>
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="B191" t="s">
-        <v>836</v>
+        <v>831</v>
       </c>
       <c r="D191" t="s">
-        <v>843</v>
+        <v>838</v>
       </c>
       <c r="F191" t="s">
-        <v>851</v>
+        <v>846</v>
       </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="B192" t="s">
-        <v>837</v>
+        <v>832</v>
       </c>
       <c r="D192" t="s">
-        <v>844</v>
+        <v>839</v>
       </c>
       <c r="F192" t="s">
-        <v>852</v>
+        <v>847</v>
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B193" t="s">
-        <v>838</v>
+        <v>833</v>
       </c>
       <c r="D193" t="s">
-        <v>845</v>
+        <v>840</v>
       </c>
       <c r="F193" t="s">
-        <v>853</v>
+        <v>848</v>
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="B194" t="s">
-        <v>839</v>
+        <v>834</v>
       </c>
       <c r="D194" t="s">
-        <v>846</v>
+        <v>841</v>
       </c>
       <c r="F194" t="s">
-        <v>854</v>
+        <v>849</v>
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B195" t="s">
-        <v>833</v>
+        <v>828</v>
       </c>
       <c r="D195" t="s">
-        <v>847</v>
+        <v>842</v>
       </c>
       <c r="F195" t="s">
-        <v>855</v>
+        <v>850</v>
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="B196" t="s">
-        <v>840</v>
+        <v>835</v>
       </c>
       <c r="D196" t="s">
-        <v>848</v>
+        <v>843</v>
       </c>
       <c r="F196" t="s">
-        <v>856</v>
+        <v>851</v>
       </c>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
+        <v>663</v>
+      </c>
+      <c r="B199" t="s">
         <v>664</v>
       </c>
-      <c r="B199" t="s">
+      <c r="D199" t="s">
         <v>665</v>
       </c>
-      <c r="D199" t="s">
-        <v>666</v>
-      </c>
       <c r="F199" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
+        <v>666</v>
+      </c>
+      <c r="B200" t="s">
         <v>667</v>
       </c>
-      <c r="B200" t="s">
+      <c r="D200" t="s">
         <v>668</v>
       </c>
-      <c r="D200" t="s">
+      <c r="F200" t="s">
         <v>669</v>
-      </c>
-      <c r="F200" t="s">
-        <v>670</v>
       </c>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
+        <v>670</v>
+      </c>
+      <c r="B201" t="s">
         <v>671</v>
       </c>
-      <c r="B201" t="s">
+      <c r="D201" t="s">
         <v>672</v>
       </c>
-      <c r="D201" t="s">
-        <v>673</v>
-      </c>
       <c r="F201" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
+        <v>673</v>
+      </c>
+      <c r="B202" t="s">
         <v>674</v>
       </c>
-      <c r="B202" t="s">
-        <v>675</v>
-      </c>
       <c r="D202" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="F202" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
+        <v>675</v>
+      </c>
+      <c r="B203" t="s">
         <v>676</v>
       </c>
-      <c r="B203" t="s">
+      <c r="D203" t="s">
         <v>677</v>
       </c>
-      <c r="D203" t="s">
-        <v>678</v>
-      </c>
       <c r="F203" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
+        <v>678</v>
+      </c>
+      <c r="B204" t="s">
         <v>679</v>
       </c>
-      <c r="B204" t="s">
+      <c r="D204" t="s">
         <v>680</v>
       </c>
-      <c r="D204" t="s">
-        <v>681</v>
-      </c>
       <c r="F204" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
+        <v>681</v>
+      </c>
+      <c r="B205" t="s">
         <v>682</v>
       </c>
-      <c r="B205" t="s">
+      <c r="D205" t="s">
         <v>683</v>
       </c>
-      <c r="D205" t="s">
-        <v>684</v>
-      </c>
       <c r="F205" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
+        <v>684</v>
+      </c>
+      <c r="B206" t="s">
         <v>685</v>
       </c>
-      <c r="B206" t="s">
+      <c r="D206" t="s">
         <v>686</v>
       </c>
-      <c r="D206" t="s">
-        <v>687</v>
-      </c>
       <c r="F206" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
+        <v>687</v>
+      </c>
+      <c r="B207" t="s">
         <v>688</v>
       </c>
-      <c r="B207" t="s">
+      <c r="D207" t="s">
         <v>689</v>
       </c>
-      <c r="D207" t="s">
-        <v>690</v>
-      </c>
       <c r="F207" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
+        <v>690</v>
+      </c>
+      <c r="B208" t="s">
         <v>691</v>
       </c>
-      <c r="B208" t="s">
+      <c r="D208" t="s">
         <v>692</v>
       </c>
-      <c r="D208" t="s">
+      <c r="F208" t="s">
         <v>693</v>
-      </c>
-      <c r="F208" t="s">
-        <v>694</v>
       </c>
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
+        <v>694</v>
+      </c>
+      <c r="B209" t="s">
         <v>695</v>
       </c>
-      <c r="B209" t="s">
+      <c r="D209" t="s">
         <v>696</v>
       </c>
-      <c r="D209" t="s">
+      <c r="F209" t="s">
         <v>697</v>
-      </c>
-      <c r="F209" t="s">
-        <v>698</v>
       </c>
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
+        <v>698</v>
+      </c>
+      <c r="B210" t="s">
         <v>699</v>
       </c>
-      <c r="B210" t="s">
+      <c r="D210" t="s">
         <v>700</v>
       </c>
-      <c r="D210" t="s">
-        <v>701</v>
-      </c>
       <c r="F210" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
+        <v>701</v>
+      </c>
+      <c r="B211" t="s">
         <v>702</v>
       </c>
-      <c r="B211" t="s">
+      <c r="D211" t="s">
         <v>703</v>
       </c>
-      <c r="D211" t="s">
-        <v>704</v>
-      </c>
       <c r="F211" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
+        <v>704</v>
+      </c>
+      <c r="B212" t="s">
         <v>705</v>
       </c>
-      <c r="B212" t="s">
+      <c r="D212" t="s">
         <v>706</v>
       </c>
-      <c r="D212" t="s">
-        <v>707</v>
-      </c>
       <c r="F212" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
+        <v>707</v>
+      </c>
+      <c r="B213" t="s">
         <v>708</v>
       </c>
-      <c r="B213" t="s">
+      <c r="D213" t="s">
         <v>709</v>
       </c>
-      <c r="D213" t="s">
+      <c r="F213" t="s">
         <v>710</v>
-      </c>
-      <c r="F213" t="s">
-        <v>711</v>
       </c>
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
+        <v>711</v>
+      </c>
+      <c r="B214" t="s">
         <v>712</v>
       </c>
-      <c r="B214" t="s">
+      <c r="D214" t="s">
         <v>713</v>
       </c>
-      <c r="D214" t="s">
+      <c r="F214" t="s">
         <v>714</v>
-      </c>
-      <c r="F214" t="s">
-        <v>715</v>
       </c>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
+        <v>715</v>
+      </c>
+      <c r="B215" t="s">
         <v>716</v>
       </c>
-      <c r="B215" t="s">
+      <c r="D215" t="s">
         <v>717</v>
       </c>
-      <c r="D215" t="s">
+      <c r="F215" t="s">
         <v>718</v>
-      </c>
-      <c r="F215" t="s">
-        <v>719</v>
       </c>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
+        <v>719</v>
+      </c>
+      <c r="B216" t="s">
         <v>720</v>
       </c>
-      <c r="B216" t="s">
+      <c r="D216" t="s">
         <v>721</v>
       </c>
-      <c r="D216" t="s">
-        <v>722</v>
-      </c>
       <c r="F216" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
+        <v>722</v>
+      </c>
+      <c r="B217" t="s">
         <v>723</v>
       </c>
-      <c r="B217" t="s">
+      <c r="D217" t="s">
         <v>724</v>
       </c>
-      <c r="D217" t="s">
+      <c r="F217" t="s">
         <v>725</v>
-      </c>
-      <c r="F217" t="s">
-        <v>726</v>
       </c>
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
+        <v>726</v>
+      </c>
+      <c r="B218" t="s">
         <v>727</v>
       </c>
-      <c r="B218" t="s">
+      <c r="D218" t="s">
         <v>728</v>
       </c>
-      <c r="D218" t="s">
+      <c r="F218" t="s">
         <v>729</v>
-      </c>
-      <c r="F218" t="s">
-        <v>730</v>
       </c>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
+        <v>730</v>
+      </c>
+      <c r="B219" t="s">
         <v>731</v>
       </c>
-      <c r="B219" t="s">
+      <c r="D219" t="s">
         <v>732</v>
       </c>
-      <c r="D219" t="s">
+      <c r="F219" t="s">
         <v>733</v>
-      </c>
-      <c r="F219" t="s">
-        <v>734</v>
       </c>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
+        <v>734</v>
+      </c>
+      <c r="B220" t="s">
         <v>735</v>
       </c>
-      <c r="B220" t="s">
+      <c r="D220" t="s">
         <v>736</v>
       </c>
-      <c r="D220" t="s">
+      <c r="F220" t="s">
         <v>737</v>
-      </c>
-      <c r="F220" t="s">
-        <v>738</v>
       </c>
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
+        <v>738</v>
+      </c>
+      <c r="B221" t="s">
         <v>739</v>
       </c>
-      <c r="B221" t="s">
+      <c r="D221" t="s">
         <v>740</v>
       </c>
-      <c r="D221" t="s">
+      <c r="F221" t="s">
         <v>741</v>
-      </c>
-      <c r="F221" t="s">
-        <v>742</v>
       </c>
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
+        <v>742</v>
+      </c>
+      <c r="B222" t="s">
         <v>743</v>
       </c>
-      <c r="B222" t="s">
+      <c r="D222" t="s">
         <v>744</v>
       </c>
-      <c r="D222" t="s">
-        <v>745</v>
-      </c>
       <c r="F222" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
+        <v>745</v>
+      </c>
+      <c r="B223" t="s">
         <v>746</v>
       </c>
-      <c r="B223" t="s">
+      <c r="D223" t="s">
         <v>747</v>
       </c>
-      <c r="D223" t="s">
-        <v>748</v>
-      </c>
       <c r="F223" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
+        <v>748</v>
+      </c>
+      <c r="B225" t="s">
         <v>749</v>
       </c>
-      <c r="B225" t="s">
+      <c r="D225" t="s">
         <v>750</v>
       </c>
-      <c r="D225" t="s">
-        <v>751</v>
-      </c>
       <c r="F225" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
+        <v>751</v>
+      </c>
+      <c r="B226" t="s">
         <v>752</v>
       </c>
-      <c r="B226" t="s">
+      <c r="D226" t="s">
         <v>753</v>
       </c>
-      <c r="D226" t="s">
-        <v>754</v>
-      </c>
       <c r="F226" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
+        <v>754</v>
+      </c>
+      <c r="B227" t="s">
         <v>755</v>
       </c>
-      <c r="B227" t="s">
+      <c r="D227" t="s">
         <v>756</v>
       </c>
-      <c r="D227" t="s">
-        <v>757</v>
-      </c>
       <c r="F227" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
+        <v>757</v>
+      </c>
+      <c r="B228" t="s">
         <v>758</v>
       </c>
-      <c r="B228" t="s">
+      <c r="D228" t="s">
         <v>759</v>
       </c>
-      <c r="D228" t="s">
-        <v>760</v>
-      </c>
       <c r="F228" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
+        <v>760</v>
+      </c>
+      <c r="B229" t="s">
         <v>761</v>
       </c>
-      <c r="B229" t="s">
+      <c r="D229" t="s">
         <v>762</v>
       </c>
-      <c r="D229" t="s">
-        <v>763</v>
-      </c>
       <c r="F229" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
+        <v>763</v>
+      </c>
+      <c r="B230" t="s">
         <v>764</v>
       </c>
-      <c r="B230" t="s">
+      <c r="D230" t="s">
         <v>765</v>
       </c>
-      <c r="D230" t="s">
-        <v>766</v>
-      </c>
       <c r="F230" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
+        <v>766</v>
+      </c>
+      <c r="B231" t="s">
         <v>767</v>
       </c>
-      <c r="B231" t="s">
+      <c r="D231" t="s">
         <v>768</v>
       </c>
-      <c r="D231" t="s">
-        <v>769</v>
-      </c>
       <c r="F231" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
+        <v>769</v>
+      </c>
+      <c r="B232" t="s">
         <v>770</v>
       </c>
-      <c r="B232" t="s">
+      <c r="D232" t="s">
         <v>771</v>
       </c>
-      <c r="D232" t="s">
-        <v>772</v>
-      </c>
       <c r="F232" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
+        <v>772</v>
+      </c>
+      <c r="B233" t="s">
         <v>773</v>
       </c>
-      <c r="B233" t="s">
+      <c r="D233" t="s">
         <v>774</v>
       </c>
-      <c r="D233" t="s">
-        <v>775</v>
-      </c>
       <c r="F233" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
+        <v>775</v>
+      </c>
+      <c r="B234" t="s">
         <v>776</v>
       </c>
-      <c r="B234" t="s">
+      <c r="D234" t="s">
         <v>777</v>
       </c>
-      <c r="D234" t="s">
-        <v>778</v>
-      </c>
       <c r="F234" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
+        <v>778</v>
+      </c>
+      <c r="B235" t="s">
         <v>779</v>
       </c>
-      <c r="B235" t="s">
+      <c r="D235" t="s">
         <v>780</v>
       </c>
-      <c r="D235" t="s">
+      <c r="F235" t="s">
         <v>781</v>
-      </c>
-      <c r="F235" t="s">
-        <v>782</v>
       </c>
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
+        <v>782</v>
+      </c>
+      <c r="B237" t="s">
         <v>783</v>
       </c>
-      <c r="B237" t="s">
+      <c r="D237" t="s">
         <v>784</v>
       </c>
-      <c r="D237" t="s">
-        <v>785</v>
-      </c>
       <c r="F237" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
+        <v>785</v>
+      </c>
+      <c r="B238" t="s">
         <v>786</v>
       </c>
-      <c r="B238" t="s">
+      <c r="D238" t="s">
         <v>787</v>
       </c>
-      <c r="D238" t="s">
+      <c r="F238" t="s">
         <v>788</v>
-      </c>
-      <c r="F238" t="s">
-        <v>789</v>
       </c>
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
+        <v>789</v>
+      </c>
+      <c r="B240" t="s">
+        <v>789</v>
+      </c>
+      <c r="D240" t="s">
         <v>790</v>
       </c>
-      <c r="B240" t="s">
-        <v>790</v>
-      </c>
-      <c r="D240" t="s">
+      <c r="F240" t="s">
         <v>791</v>
-      </c>
-      <c r="F240" t="s">
-        <v>792</v>
       </c>
     </row>
     <row r="241" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
+        <v>792</v>
+      </c>
+      <c r="B241" t="s">
+        <v>792</v>
+      </c>
+      <c r="D241" t="s">
         <v>793</v>
       </c>
-      <c r="B241" t="s">
-        <v>793</v>
-      </c>
-      <c r="D241" t="s">
+      <c r="F241" t="s">
         <v>794</v>
-      </c>
-      <c r="F241" t="s">
-        <v>795</v>
       </c>
     </row>
     <row r="242" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
+        <v>795</v>
+      </c>
+      <c r="B242" t="s">
+        <v>795</v>
+      </c>
+      <c r="D242" t="s">
         <v>796</v>
       </c>
-      <c r="B242" t="s">
-        <v>796</v>
-      </c>
-      <c r="D242" t="s">
+      <c r="F242" t="s">
         <v>797</v>
-      </c>
-      <c r="F242" t="s">
-        <v>798</v>
       </c>
     </row>
     <row r="243" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
+        <v>798</v>
+      </c>
+      <c r="B243" t="s">
+        <v>798</v>
+      </c>
+      <c r="D243" t="s">
         <v>799</v>
       </c>
-      <c r="B243" t="s">
-        <v>799</v>
-      </c>
-      <c r="D243" t="s">
+      <c r="F243" t="s">
         <v>800</v>
-      </c>
-      <c r="F243" t="s">
-        <v>801</v>
       </c>
     </row>
     <row r="244" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="B244" t="s">
+        <v>792</v>
+      </c>
+      <c r="D244" t="s">
         <v>793</v>
       </c>
-      <c r="D244" t="s">
+      <c r="F244" t="s">
         <v>794</v>
-      </c>
-      <c r="F244" t="s">
-        <v>795</v>
       </c>
     </row>
     <row r="245" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="B245" t="s">
+        <v>795</v>
+      </c>
+      <c r="D245" t="s">
         <v>796</v>
       </c>
-      <c r="D245" t="s">
+      <c r="F245" t="s">
         <v>797</v>
-      </c>
-      <c r="F245" t="s">
-        <v>798</v>
       </c>
     </row>
     <row r="246" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="B246" t="s">
+        <v>798</v>
+      </c>
+      <c r="D246" t="s">
         <v>799</v>
       </c>
-      <c r="D246" t="s">
+      <c r="F246" t="s">
         <v>800</v>
-      </c>
-      <c r="F246" t="s">
-        <v>801</v>
       </c>
     </row>
     <row r="247" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="B247" t="s">
-        <v>408</v>
+        <v>804</v>
       </c>
       <c r="D247" t="s">
-        <v>409</v>
+        <v>857</v>
       </c>
       <c r="F247" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
     </row>
     <row r="248" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B248" t="s">
-        <v>807</v>
+        <v>856</v>
       </c>
       <c r="D248" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="F248" t="s">
-        <v>808</v>
+        <v>859</v>
       </c>
     </row>
     <row r="249" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="B249" t="s">
-        <v>810</v>
+        <v>807</v>
+      </c>
+      <c r="D249" t="s">
+        <v>854</v>
       </c>
       <c r="F249" t="s">
-        <v>811</v>
+        <v>806</v>
       </c>
     </row>
     <row r="250" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
-        <v>812</v>
+        <v>808</v>
       </c>
       <c r="B250" t="s">
-        <v>813</v>
+        <v>809</v>
+      </c>
+      <c r="D250" t="s">
+        <v>855</v>
       </c>
       <c r="F250" t="s">
-        <v>814</v>
+        <v>808</v>
       </c>
     </row>
     <row r="252" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
-        <v>815</v>
+        <v>810</v>
       </c>
       <c r="B252" t="s">
-        <v>815</v>
+        <v>810</v>
       </c>
       <c r="D252" t="s">
-        <v>815</v>
+        <v>810</v>
       </c>
       <c r="F252" t="s">
-        <v>815</v>
+        <v>810</v>
       </c>
     </row>
     <row r="253" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
-        <v>816</v>
+        <v>811</v>
       </c>
       <c r="B253" t="s">
-        <v>816</v>
+        <v>811</v>
       </c>
       <c r="D253" t="s">
-        <v>816</v>
+        <v>811</v>
       </c>
       <c r="F253" t="s">
-        <v>816</v>
+        <v>811</v>
       </c>
     </row>
     <row r="254" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
-        <v>817</v>
+        <v>812</v>
       </c>
       <c r="B254" t="s">
-        <v>817</v>
+        <v>812</v>
       </c>
       <c r="D254" t="s">
-        <v>817</v>
+        <v>812</v>
       </c>
       <c r="F254" t="s">
-        <v>817</v>
+        <v>812</v>
       </c>
     </row>
     <row r="255" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
-        <v>818</v>
+        <v>813</v>
       </c>
       <c r="B255" t="s">
-        <v>818</v>
+        <v>813</v>
       </c>
       <c r="D255" t="s">
-        <v>818</v>
+        <v>813</v>
       </c>
       <c r="F255" t="s">
-        <v>818</v>
+        <v>813</v>
       </c>
     </row>
     <row r="256" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
-        <v>819</v>
+        <v>814</v>
       </c>
       <c r="B256" t="s">
-        <v>819</v>
+        <v>814</v>
       </c>
       <c r="D256" t="s">
-        <v>819</v>
+        <v>814</v>
       </c>
       <c r="F256" t="s">
-        <v>819</v>
+        <v>814</v>
       </c>
     </row>
     <row r="257" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
-        <v>820</v>
+        <v>815</v>
       </c>
       <c r="B257" t="s">
-        <v>820</v>
+        <v>815</v>
       </c>
       <c r="D257" t="s">
-        <v>820</v>
+        <v>815</v>
       </c>
       <c r="F257" t="s">
-        <v>820</v>
+        <v>815</v>
       </c>
     </row>
     <row r="258" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
-        <v>821</v>
+        <v>816</v>
       </c>
       <c r="B258" t="s">
-        <v>821</v>
+        <v>816</v>
       </c>
       <c r="D258" t="s">
-        <v>821</v>
+        <v>816</v>
       </c>
       <c r="F258" t="s">
-        <v>821</v>
+        <v>816</v>
       </c>
     </row>
     <row r="259" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
-        <v>822</v>
+        <v>817</v>
       </c>
       <c r="B259" t="s">
-        <v>822</v>
+        <v>817</v>
       </c>
       <c r="D259" t="s">
-        <v>822</v>
+        <v>817</v>
       </c>
       <c r="F259" t="s">
-        <v>822</v>
+        <v>817</v>
       </c>
     </row>
     <row r="260" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
-        <v>823</v>
+        <v>818</v>
       </c>
       <c r="B260" t="s">
-        <v>823</v>
+        <v>818</v>
       </c>
       <c r="D260" t="s">
-        <v>823</v>
+        <v>818</v>
       </c>
       <c r="F260" t="s">
-        <v>823</v>
+        <v>818</v>
       </c>
     </row>
     <row r="261" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
-        <v>824</v>
+        <v>819</v>
       </c>
       <c r="B261" t="s">
-        <v>824</v>
+        <v>819</v>
       </c>
       <c r="D261" t="s">
-        <v>824</v>
+        <v>819</v>
       </c>
       <c r="F261" t="s">
-        <v>824</v>
+        <v>819</v>
       </c>
     </row>
     <row r="263" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
-        <v>825</v>
+        <v>820</v>
       </c>
       <c r="B263" t="s">
-        <v>826</v>
+        <v>821</v>
+      </c>
+      <c r="D263" t="s">
+        <v>860</v>
+      </c>
+      <c r="F263" t="s">
+        <v>864</v>
       </c>
     </row>
     <row r="264" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
-        <v>827</v>
+        <v>822</v>
       </c>
       <c r="B264" t="s">
-        <v>828</v>
+        <v>823</v>
+      </c>
+      <c r="D264" t="s">
+        <v>861</v>
+      </c>
+      <c r="F264" t="s">
+        <v>865</v>
       </c>
     </row>
     <row r="265" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
-        <v>829</v>
+        <v>824</v>
       </c>
       <c r="B265" t="s">
-        <v>830</v>
+        <v>825</v>
+      </c>
+      <c r="D265" t="s">
+        <v>862</v>
+      </c>
+      <c r="F265" t="s">
+        <v>862</v>
       </c>
     </row>
     <row r="266" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
-        <v>831</v>
+        <v>826</v>
       </c>
       <c r="B266" t="s">
-        <v>832</v>
+        <v>827</v>
+      </c>
+      <c r="D266" t="s">
+        <v>863</v>
+      </c>
+      <c r="F266" t="s">
+        <v>863</v>
       </c>
     </row>
   </sheetData>

</xml_diff>